<commit_message>
row index fix and removed extra spaces from table
</commit_message>
<xml_diff>
--- a/test_files/test1_excel.xlsx
+++ b/test_files/test1_excel.xlsx
@@ -4,24 +4,34 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="5">
   <si>
     <t>Name</t>
   </si>
   <si>
     <t>TESTFILE1</t>
+  </si>
+  <si>
+    <t>sheet4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B COL </t>
+  </si>
+  <si>
+    <t>C COL</t>
   </si>
 </sst>
 </file>
@@ -355,8 +365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -393,6 +403,145 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A6:D16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="4" max="4" width="19.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
added row index for both and loading spinner
</commit_message>
<xml_diff>
--- a/test_files/test1_excel.xlsx
+++ b/test_files/test1_excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -32,6 +32,21 @@
   </si>
   <si>
     <t>C COL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dffffffffffffffffff fh uhurhguhgh u  htri hg  hri ri hg  I hgi hri hrgir hgihrighsrigrs </t>
+  </si>
+  <si>
+    <t>sdd</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>fdf jfij ji  ij  jij  jijfijf jfijfi j jdfithe u ie hfdf jfij ji  ij  jij  jijfijf jfijfi j jdfithe u ie h fdf jfij ji  ij  jij  jijfijf jfijfi j jdfithe u ie hfdf jfij ji  ij  jij  jijfijf jfijfi j jdfithe u ie hfdf jfij ji  ij  jij  jijfijf jfijfi j jdfithe u ie hfdf jfij ji  ij  jij  jijfijf jfijfi j jdfithe u ie hfdf jfij ji  ij  jij  jijfijf jfijfi j jdfithe u ie hfdf jfij ji  ij  jij  jijfijf jfijfi j jdfithe u ie hfdf jfij ji  ij  jij  jijfijf jfijfi j jdfithe u ie hfdf jfij ji  ij  jij  jijfijf jfijfi j jdfithe u ie hfdf jfij ji  ij  jij  jijfijf jfijfi j jdfithe u ie hfdf jfij ji  ij  jij  jijfijf jfijfi j jdfithe u ie hfdf jfij ji  ij  jij  jijfijf jfijfi j jdfithe u ie hfdf jfij ji  ij  jij  jijfijf jfijfi j jdfithe u ie hfdf jfij ji  ij  jij  jijfijf jfijfi j jdfithe u ie h</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -363,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -382,6 +397,16 @@
     <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -403,10 +428,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A6:D16"/>
+  <dimension ref="A6:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -533,6 +558,36 @@
       </c>
       <c r="D16" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>